<commit_message>
Added costs for cards
</commit_message>
<xml_diff>
--- a/data/Dominion Cards.xlsx
+++ b/data/Dominion Cards.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kosht\Documents\Dominion\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kosht\Documents\Dominion\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{98866413-BE96-4CFC-8D57-26473C7ACBAD}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{983FBE70-A9F0-4EE4-A6AF-BD58F12A37FF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660" activeTab="1" xr2:uid="{63D99CEF-D166-4221-8053-429A0416F649}"/>
   </bookViews>
@@ -18,7 +18,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'ALL CARDS'!$A$1:$B$1305</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Owned!$A$1:$B$588</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Owned!$A$1:$C$165</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1560" uniqueCount="607">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1507" uniqueCount="609">
   <si>
     <t>Base</t>
   </si>
@@ -1851,6 +1851,12 @@
   </si>
   <si>
     <t>Wharf</t>
+  </si>
+  <si>
+    <t>Cost</t>
+  </si>
+  <si>
+    <t>Knights</t>
   </si>
 </sst>
 </file>
@@ -2221,7 +2227,7 @@
   <dimension ref="A1:J1305"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="A1:B588"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -8910,10 +8916,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69730851-B1B4-4793-A306-A6AD37F5E4E5}">
-  <dimension ref="A1:B588"/>
+  <dimension ref="A1:C566"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView tabSelected="1" topLeftCell="A147" workbookViewId="0">
+      <selection activeCell="D156" sqref="D156"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -8922,1541 +8928,1874 @@
     <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>23</v>
       </c>
       <c r="B1" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C1" t="s">
+        <v>607</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>20</v>
       </c>
       <c r="B2" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>21</v>
       </c>
       <c r="B3" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>22</v>
       </c>
       <c r="B4" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>96</v>
       </c>
       <c r="B5" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>97</v>
       </c>
       <c r="B6" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>98</v>
       </c>
       <c r="B7" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C7">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
         <v>99</v>
       </c>
       <c r="B8" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C8">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>100</v>
       </c>
       <c r="B9" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C9">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>101</v>
       </c>
       <c r="B10" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C10">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
         <v>102</v>
       </c>
       <c r="B11" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C11">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
         <v>103</v>
       </c>
       <c r="B12" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C12">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
         <v>104</v>
       </c>
       <c r="B13" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C13">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
         <v>105</v>
       </c>
       <c r="B14" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C14">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
         <v>106</v>
       </c>
       <c r="B15" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C15">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
         <v>107</v>
       </c>
       <c r="B16" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C16">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
         <v>108</v>
       </c>
       <c r="B17" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C17">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A18" s="1" t="s">
         <v>109</v>
       </c>
       <c r="B18" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C18">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A19" s="1" t="s">
         <v>110</v>
       </c>
       <c r="B19" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C19">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>111</v>
       </c>
       <c r="B20" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C20">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A21" s="1" t="s">
         <v>124</v>
       </c>
       <c r="B21" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C21">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>125</v>
       </c>
       <c r="B22" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C22">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>126</v>
       </c>
       <c r="B23" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C23">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A24" s="1" t="s">
         <v>127</v>
       </c>
       <c r="B24" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C24">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A25" s="1" t="s">
         <v>128</v>
       </c>
       <c r="B25" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>129</v>
       </c>
       <c r="B26" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C26">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>130</v>
       </c>
       <c r="B27" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C27">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>131</v>
       </c>
       <c r="B28" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C28">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A29" s="1" t="s">
         <v>132</v>
       </c>
       <c r="B29" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C29">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A30" s="1" t="s">
         <v>18</v>
       </c>
       <c r="B30" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C30">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>133</v>
       </c>
       <c r="B31" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C31">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A32" s="1" t="s">
         <v>134</v>
       </c>
       <c r="B32" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C32">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A33" s="1" t="s">
         <v>135</v>
       </c>
       <c r="B33" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C33">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A34" s="1" t="s">
         <v>136</v>
       </c>
       <c r="B34" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C34">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A35" s="1" t="s">
         <v>137</v>
       </c>
       <c r="B35" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C35">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>138</v>
       </c>
       <c r="B36" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C36">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A37" s="1" t="s">
         <v>139</v>
       </c>
       <c r="B37" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C37">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A38" s="1" t="s">
         <v>140</v>
       </c>
       <c r="B38" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C38">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A39" s="1" t="s">
         <v>141</v>
       </c>
       <c r="B39" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C39">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A40" s="1" t="s">
         <v>142</v>
       </c>
       <c r="B40" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C40">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A41" s="1" t="s">
-        <v>143</v>
+        <v>148</v>
       </c>
       <c r="B41" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.35">
+        <v>12</v>
+      </c>
+      <c r="C41">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A42" s="1" t="s">
-        <v>144</v>
+        <v>149</v>
       </c>
       <c r="B42" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.35">
+        <v>12</v>
+      </c>
+      <c r="C42">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A43" s="1" t="s">
-        <v>145</v>
+        <v>150</v>
       </c>
       <c r="B43" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.35">
+        <v>12</v>
+      </c>
+      <c r="C43">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A44" s="1" t="s">
-        <v>146</v>
+        <v>151</v>
       </c>
       <c r="B44" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A45" s="1" t="s">
-        <v>147</v>
+        <v>12</v>
+      </c>
+      <c r="C44">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A45" t="s">
+        <v>152</v>
       </c>
       <c r="B45" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A46" s="1" t="s">
-        <v>148</v>
+        <v>12</v>
+      </c>
+      <c r="C45">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A46" t="s">
+        <v>153</v>
       </c>
       <c r="B46" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C46">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A47" s="1" t="s">
-        <v>149</v>
+        <v>154</v>
       </c>
       <c r="B47" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C47">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A48" s="1" t="s">
-        <v>150</v>
+        <v>155</v>
       </c>
       <c r="B48" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A49" s="1" t="s">
-        <v>151</v>
+      <c r="C48">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A49" t="s">
+        <v>156</v>
       </c>
       <c r="B49" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A50" t="s">
-        <v>152</v>
+      <c r="C49">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A50" s="1" t="s">
+        <v>157</v>
       </c>
       <c r="B50" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A51" t="s">
-        <v>153</v>
+      <c r="C50">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A51" s="1" t="s">
+        <v>158</v>
       </c>
       <c r="B51" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A52" s="1" t="s">
-        <v>154</v>
+      <c r="C51">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A52" t="s">
+        <v>159</v>
       </c>
       <c r="B52" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C52">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A53" s="1" t="s">
-        <v>155</v>
+        <v>160</v>
       </c>
       <c r="B53" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A54" t="s">
-        <v>156</v>
+      <c r="C53">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A54" s="1" t="s">
+        <v>161</v>
       </c>
       <c r="B54" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A55" s="1" t="s">
-        <v>157</v>
+      <c r="C54">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A55" t="s">
+        <v>162</v>
       </c>
       <c r="B55" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C55">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A56" s="1" t="s">
-        <v>158</v>
+        <v>163</v>
       </c>
       <c r="B56" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A57" t="s">
-        <v>159</v>
+      <c r="C56">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A57" s="1" t="s">
+        <v>164</v>
       </c>
       <c r="B57" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C57">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A58" s="1" t="s">
-        <v>160</v>
+        <v>165</v>
       </c>
       <c r="B58" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C58">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A59" s="1" t="s">
-        <v>161</v>
+        <v>166</v>
       </c>
       <c r="B59" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C59">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
-        <v>162</v>
+        <v>167</v>
       </c>
       <c r="B60" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C60">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A61" s="1" t="s">
-        <v>163</v>
+        <v>168</v>
       </c>
       <c r="B61" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C61">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A62" s="1" t="s">
-        <v>164</v>
+        <v>169</v>
       </c>
       <c r="B62" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A63" s="1" t="s">
-        <v>165</v>
+      <c r="C62">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A63" t="s">
+        <v>170</v>
       </c>
       <c r="B63" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A64" s="1" t="s">
-        <v>166</v>
+      <c r="C63">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A64" t="s">
+        <v>171</v>
       </c>
       <c r="B64" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A65" t="s">
-        <v>167</v>
+      <c r="C64">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A65" s="1" t="s">
+        <v>172</v>
       </c>
       <c r="B65" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C65">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A66" s="1" t="s">
-        <v>168</v>
+        <v>173</v>
       </c>
       <c r="B66" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C66">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A67" s="1" t="s">
-        <v>169</v>
+        <v>174</v>
       </c>
       <c r="B67" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A68" t="s">
-        <v>170</v>
+      <c r="C67">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A68" s="1" t="s">
+        <v>175</v>
       </c>
       <c r="B68" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A69" t="s">
-        <v>171</v>
+      <c r="C68">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A69" s="1" t="s">
+        <v>608</v>
       </c>
       <c r="B69" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A70" s="1" t="s">
-        <v>172</v>
+      <c r="C69">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A70" t="s">
+        <v>176</v>
       </c>
       <c r="B70" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C70">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A71" s="1" t="s">
-        <v>173</v>
+        <v>177</v>
       </c>
       <c r="B71" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C71">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A72" s="1" t="s">
-        <v>174</v>
+        <v>178</v>
       </c>
       <c r="B72" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C72">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A73" s="1" t="s">
-        <v>175</v>
+        <v>179</v>
       </c>
       <c r="B73" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C73">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
-        <v>176</v>
+        <v>180</v>
       </c>
       <c r="B74" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C74">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A75" s="1" t="s">
-        <v>177</v>
+        <v>181</v>
       </c>
       <c r="B75" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C75">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A76" s="1" t="s">
-        <v>178</v>
+        <v>273</v>
       </c>
       <c r="B76" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A77" s="1" t="s">
-        <v>179</v>
+        <v>13</v>
+      </c>
+      <c r="C76">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A77" t="s">
+        <v>274</v>
       </c>
       <c r="B77" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A78" t="s">
-        <v>180</v>
+        <v>13</v>
+      </c>
+      <c r="C77">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A78" s="1" t="s">
+        <v>275</v>
       </c>
       <c r="B78" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.35">
+        <v>13</v>
+      </c>
+      <c r="C78">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A79" s="1" t="s">
-        <v>181</v>
+        <v>276</v>
       </c>
       <c r="B79" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.35">
+        <v>13</v>
+      </c>
+      <c r="C79">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A80" s="1" t="s">
-        <v>182</v>
+        <v>277</v>
       </c>
       <c r="B80" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A81" s="1" t="s">
-        <v>183</v>
+        <v>13</v>
+      </c>
+      <c r="C80">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A81" t="s">
+        <v>278</v>
       </c>
       <c r="B81" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.35">
+        <v>13</v>
+      </c>
+      <c r="C81">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A82" s="1" t="s">
-        <v>184</v>
+        <v>279</v>
       </c>
       <c r="B82" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.35">
+        <v>13</v>
+      </c>
+      <c r="C82">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A83" s="1" t="s">
-        <v>185</v>
+        <v>280</v>
       </c>
       <c r="B83" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A84" t="s">
-        <v>186</v>
+        <v>13</v>
+      </c>
+      <c r="C83">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A84" s="1" t="s">
+        <v>281</v>
       </c>
       <c r="B84" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.35">
+        <v>13</v>
+      </c>
+      <c r="C84">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A85" s="1" t="s">
-        <v>187</v>
+        <v>282</v>
       </c>
       <c r="B85" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.35">
+        <v>13</v>
+      </c>
+      <c r="C85">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A86" s="1" t="s">
-        <v>188</v>
+        <v>283</v>
       </c>
       <c r="B86" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A87" t="s">
-        <v>189</v>
+        <v>13</v>
+      </c>
+      <c r="C86">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A87" s="1" t="s">
+        <v>284</v>
       </c>
       <c r="B87" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A88" s="1" t="s">
-        <v>190</v>
+        <v>13</v>
+      </c>
+      <c r="C87">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A88" t="s">
+        <v>285</v>
       </c>
       <c r="B88" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A89" s="1" t="s">
-        <v>191</v>
+        <v>13</v>
+      </c>
+      <c r="C88">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A89" t="s">
+        <v>312</v>
       </c>
       <c r="B89" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.35">
+        <v>4</v>
+      </c>
+      <c r="C89">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A90" s="1" t="s">
-        <v>192</v>
+        <v>313</v>
       </c>
       <c r="B90" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.35">
+        <v>4</v>
+      </c>
+      <c r="C90">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A91" s="1" t="s">
-        <v>193</v>
+        <v>314</v>
       </c>
       <c r="B91" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A92" t="s">
-        <v>194</v>
+        <v>4</v>
+      </c>
+      <c r="C91">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A92" s="1" t="s">
+        <v>315</v>
       </c>
       <c r="B92" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.35">
+        <v>4</v>
+      </c>
+      <c r="C92">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A93" s="1" t="s">
-        <v>195</v>
+        <v>316</v>
       </c>
       <c r="B93" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A94" s="1" t="s">
-        <v>196</v>
+        <v>4</v>
+      </c>
+      <c r="C93">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A94" t="s">
+        <v>317</v>
       </c>
       <c r="B94" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.35">
+        <v>4</v>
+      </c>
+      <c r="C94">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A95" s="1" t="s">
-        <v>197</v>
+        <v>318</v>
       </c>
       <c r="B95" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.35">
+        <v>4</v>
+      </c>
+      <c r="C95">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A96" s="1" t="s">
-        <v>198</v>
+        <v>319</v>
       </c>
       <c r="B96" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.35">
+        <v>4</v>
+      </c>
+      <c r="C96">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A97" s="1" t="s">
-        <v>199</v>
+        <v>320</v>
       </c>
       <c r="B97" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.35">
+        <v>4</v>
+      </c>
+      <c r="C97">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A98" s="1" t="s">
-        <v>200</v>
+        <v>321</v>
       </c>
       <c r="B98" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.35">
+        <v>4</v>
+      </c>
+      <c r="C98">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A99" s="1" t="s">
-        <v>201</v>
+        <v>322</v>
       </c>
       <c r="B99" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.35">
+        <v>4</v>
+      </c>
+      <c r="C99">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A100" s="1" t="s">
-        <v>202</v>
+        <v>323</v>
       </c>
       <c r="B100" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.35">
+        <v>4</v>
+      </c>
+      <c r="C100">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A101" s="1" t="s">
-        <v>273</v>
+        <v>324</v>
       </c>
       <c r="B101" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="102" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A102" t="s">
-        <v>274</v>
+        <v>4</v>
+      </c>
+      <c r="C101">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A102" s="1" t="s">
+        <v>325</v>
       </c>
       <c r="B102" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="103" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A103" s="1" t="s">
-        <v>275</v>
+        <v>4</v>
+      </c>
+      <c r="C102">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A103" t="s">
+        <v>326</v>
       </c>
       <c r="B103" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="104" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A104" s="1" t="s">
-        <v>276</v>
+        <v>4</v>
+      </c>
+      <c r="C103">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A104" t="s">
+        <v>327</v>
       </c>
       <c r="B104" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="105" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A105" s="1" t="s">
-        <v>277</v>
+        <v>4</v>
+      </c>
+      <c r="C104">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A105" t="s">
+        <v>328</v>
       </c>
       <c r="B105" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="106" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A106" t="s">
-        <v>278</v>
+        <v>4</v>
+      </c>
+      <c r="C105">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="106" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A106" s="1" t="s">
+        <v>329</v>
       </c>
       <c r="B106" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="107" spans="1:2" x14ac:dyDescent="0.35">
+        <v>4</v>
+      </c>
+      <c r="C106">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="107" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A107" s="1" t="s">
-        <v>279</v>
+        <v>330</v>
       </c>
       <c r="B107" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="108" spans="1:2" x14ac:dyDescent="0.35">
+        <v>4</v>
+      </c>
+      <c r="C107">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="108" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A108" s="1" t="s">
-        <v>280</v>
+        <v>337</v>
       </c>
       <c r="B108" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="109" spans="1:2" x14ac:dyDescent="0.35">
+        <v>4</v>
+      </c>
+      <c r="C108">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="109" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A109" s="1" t="s">
-        <v>281</v>
+        <v>338</v>
       </c>
       <c r="B109" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="110" spans="1:2" x14ac:dyDescent="0.35">
+        <v>4</v>
+      </c>
+      <c r="C109">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="110" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A110" s="1" t="s">
-        <v>282</v>
+        <v>339</v>
       </c>
       <c r="B110" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="111" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A111" s="1" t="s">
-        <v>283</v>
+        <v>4</v>
+      </c>
+      <c r="C110">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="111" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A111" t="s">
+        <v>340</v>
       </c>
       <c r="B111" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="112" spans="1:2" x14ac:dyDescent="0.35">
+        <v>4</v>
+      </c>
+      <c r="C111">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="112" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A112" s="1" t="s">
-        <v>284</v>
+        <v>341</v>
       </c>
       <c r="B112" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="113" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A113" t="s">
-        <v>285</v>
+        <v>4</v>
+      </c>
+      <c r="C112">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="113" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A113" s="1" t="s">
+        <v>342</v>
       </c>
       <c r="B113" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="114" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A114" t="s">
-        <v>312</v>
+        <v>4</v>
+      </c>
+      <c r="C113">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="114" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A114" s="1" t="s">
+        <v>343</v>
       </c>
       <c r="B114" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="115" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C114">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="115" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A115" s="1" t="s">
-        <v>313</v>
+        <v>504</v>
       </c>
       <c r="B115" t="s">
+        <v>9</v>
+      </c>
+      <c r="C115">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="116" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A116" t="s">
+        <v>505</v>
+      </c>
+      <c r="B116" t="s">
+        <v>9</v>
+      </c>
+      <c r="C116">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="117" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A117" s="1" t="s">
+        <v>506</v>
+      </c>
+      <c r="B117" t="s">
+        <v>9</v>
+      </c>
+      <c r="C117">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="118" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A118" s="1" t="s">
+        <v>507</v>
+      </c>
+      <c r="B118" t="s">
+        <v>9</v>
+      </c>
+      <c r="C118">
         <v>4</v>
       </c>
     </row>
-    <row r="116" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A116" s="1" t="s">
-        <v>314</v>
-      </c>
-      <c r="B116" t="s">
+    <row r="119" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A119" t="s">
+        <v>508</v>
+      </c>
+      <c r="B119" t="s">
+        <v>9</v>
+      </c>
+      <c r="C119">
         <v>4</v>
       </c>
     </row>
-    <row r="117" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A117" s="1" t="s">
-        <v>315</v>
-      </c>
-      <c r="B117" t="s">
+    <row r="120" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A120" s="1" t="s">
+        <v>509</v>
+      </c>
+      <c r="B120" t="s">
+        <v>9</v>
+      </c>
+      <c r="C120">
         <v>4</v>
       </c>
     </row>
-    <row r="118" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A118" s="1" t="s">
-        <v>316</v>
-      </c>
-      <c r="B118" t="s">
+    <row r="121" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A121" s="1" t="s">
+        <v>510</v>
+      </c>
+      <c r="B121" t="s">
+        <v>9</v>
+      </c>
+      <c r="C121">
         <v>4</v>
       </c>
     </row>
-    <row r="119" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A119" t="s">
-        <v>317</v>
-      </c>
-      <c r="B119" t="s">
+    <row r="122" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A122" s="1" t="s">
+        <v>511</v>
+      </c>
+      <c r="B122" t="s">
+        <v>9</v>
+      </c>
+      <c r="C122">
         <v>4</v>
       </c>
     </row>
-    <row r="120" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A120" s="1" t="s">
-        <v>318</v>
-      </c>
-      <c r="B120" t="s">
+    <row r="123" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A123" t="s">
+        <v>512</v>
+      </c>
+      <c r="B123" t="s">
+        <v>9</v>
+      </c>
+      <c r="C123">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="124" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A124" t="s">
+        <v>513</v>
+      </c>
+      <c r="B124" t="s">
+        <v>9</v>
+      </c>
+      <c r="C124">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="125" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A125" s="1" t="s">
+        <v>514</v>
+      </c>
+      <c r="B125" t="s">
+        <v>9</v>
+      </c>
+      <c r="C125">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="126" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A126" s="1" t="s">
+        <v>515</v>
+      </c>
+      <c r="B126" t="s">
+        <v>9</v>
+      </c>
+      <c r="C126">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="127" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A127" t="s">
+        <v>516</v>
+      </c>
+      <c r="B127" t="s">
+        <v>9</v>
+      </c>
+      <c r="C127">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="128" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A128" s="1" t="s">
+        <v>517</v>
+      </c>
+      <c r="B128" t="s">
+        <v>9</v>
+      </c>
+      <c r="C128">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="129" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A129" s="1" t="s">
+        <v>518</v>
+      </c>
+      <c r="B129" t="s">
+        <v>9</v>
+      </c>
+      <c r="C129">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="130" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A130" s="1" t="s">
+        <v>519</v>
+      </c>
+      <c r="B130" t="s">
+        <v>9</v>
+      </c>
+      <c r="C130">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="131" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A131" s="1" t="s">
+        <v>520</v>
+      </c>
+      <c r="B131" t="s">
+        <v>9</v>
+      </c>
+      <c r="C131">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="132" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A132" s="1" t="s">
+        <v>521</v>
+      </c>
+      <c r="B132" t="s">
+        <v>9</v>
+      </c>
+      <c r="C132">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="133" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A133" s="1" t="s">
+        <v>522</v>
+      </c>
+      <c r="B133" t="s">
+        <v>9</v>
+      </c>
+      <c r="C133">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="134" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A134" s="1" t="s">
+        <v>523</v>
+      </c>
+      <c r="B134" t="s">
+        <v>9</v>
+      </c>
+      <c r="C134">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="135" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A135" s="1" t="s">
+        <v>524</v>
+      </c>
+      <c r="B135" t="s">
+        <v>9</v>
+      </c>
+      <c r="C135">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="136" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A136" t="s">
+        <v>525</v>
+      </c>
+      <c r="B136" t="s">
+        <v>9</v>
+      </c>
+      <c r="C136">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="137" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A137" s="1" t="s">
+        <v>526</v>
+      </c>
+      <c r="B137" t="s">
+        <v>9</v>
+      </c>
+      <c r="C137">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="138" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A138" s="1" t="s">
+        <v>527</v>
+      </c>
+      <c r="B138" t="s">
+        <v>9</v>
+      </c>
+      <c r="C138">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="139" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A139" s="1" t="s">
+        <v>528</v>
+      </c>
+      <c r="B139" t="s">
+        <v>9</v>
+      </c>
+      <c r="C139">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="140" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A140" t="s">
+        <v>581</v>
+      </c>
+      <c r="B140" t="s">
+        <v>7</v>
+      </c>
+      <c r="C140">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="141" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A141" t="s">
+        <v>582</v>
+      </c>
+      <c r="B141" t="s">
+        <v>7</v>
+      </c>
+      <c r="C141">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="142" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A142" t="s">
+        <v>583</v>
+      </c>
+      <c r="B142" t="s">
+        <v>7</v>
+      </c>
+      <c r="C142">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="143" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A143" t="s">
+        <v>584</v>
+      </c>
+      <c r="B143" t="s">
+        <v>7</v>
+      </c>
+      <c r="C143">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="144" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A144" t="s">
+        <v>585</v>
+      </c>
+      <c r="B144" t="s">
+        <v>7</v>
+      </c>
+      <c r="C144">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="145" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A145" s="1" t="s">
+        <v>586</v>
+      </c>
+      <c r="B145" t="s">
+        <v>7</v>
+      </c>
+      <c r="C145">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="146" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A146" s="1" t="s">
+        <v>587</v>
+      </c>
+      <c r="B146" t="s">
+        <v>7</v>
+      </c>
+      <c r="C146">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="147" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A147" t="s">
+        <v>588</v>
+      </c>
+      <c r="B147" t="s">
+        <v>7</v>
+      </c>
+      <c r="C147">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="148" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A148" s="1" t="s">
+        <v>589</v>
+      </c>
+      <c r="B148" t="s">
+        <v>7</v>
+      </c>
+      <c r="C148">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="149" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A149" s="1" t="s">
+        <v>590</v>
+      </c>
+      <c r="B149" t="s">
+        <v>7</v>
+      </c>
+      <c r="C149">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="150" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A150" s="1" t="s">
+        <v>591</v>
+      </c>
+      <c r="B150" t="s">
+        <v>7</v>
+      </c>
+      <c r="C150">
         <v>4</v>
       </c>
     </row>
-    <row r="121" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A121" s="1" t="s">
-        <v>319</v>
-      </c>
-      <c r="B121" t="s">
+    <row r="151" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A151" t="s">
+        <v>592</v>
+      </c>
+      <c r="B151" t="s">
+        <v>7</v>
+      </c>
+      <c r="C151">
         <v>4</v>
       </c>
     </row>
-    <row r="122" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A122" s="1" t="s">
-        <v>320</v>
-      </c>
-      <c r="B122" t="s">
+    <row r="152" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A152" t="s">
+        <v>593</v>
+      </c>
+      <c r="B152" t="s">
+        <v>7</v>
+      </c>
+      <c r="C152">
         <v>4</v>
       </c>
     </row>
-    <row r="123" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A123" s="1" t="s">
-        <v>321</v>
-      </c>
-      <c r="B123" t="s">
+    <row r="153" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A153" t="s">
+        <v>594</v>
+      </c>
+      <c r="B153" t="s">
+        <v>7</v>
+      </c>
+      <c r="C153">
         <v>4</v>
       </c>
     </row>
-    <row r="124" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A124" s="1" t="s">
-        <v>322</v>
-      </c>
-      <c r="B124" t="s">
+    <row r="154" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A154" s="1" t="s">
+        <v>595</v>
+      </c>
+      <c r="B154" t="s">
+        <v>7</v>
+      </c>
+      <c r="C154">
         <v>4</v>
       </c>
     </row>
-    <row r="125" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A125" s="1" t="s">
-        <v>323</v>
-      </c>
-      <c r="B125" t="s">
+    <row r="155" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A155" s="1" t="s">
+        <v>596</v>
+      </c>
+      <c r="B155" t="s">
+        <v>7</v>
+      </c>
+      <c r="C155">
         <v>4</v>
       </c>
     </row>
-    <row r="126" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A126" s="1" t="s">
-        <v>324</v>
-      </c>
-      <c r="B126" t="s">
+    <row r="156" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A156" s="1" t="s">
+        <v>597</v>
+      </c>
+      <c r="B156" t="s">
+        <v>7</v>
+      </c>
+      <c r="C156">
         <v>4</v>
       </c>
     </row>
-    <row r="127" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A127" s="1" t="s">
-        <v>325</v>
-      </c>
-      <c r="B127" t="s">
+    <row r="157" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A157" s="1" t="s">
+        <v>598</v>
+      </c>
+      <c r="B157" t="s">
+        <v>7</v>
+      </c>
+      <c r="C157">
         <v>4</v>
       </c>
     </row>
-    <row r="128" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A128" t="s">
-        <v>326</v>
-      </c>
-      <c r="B128" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="129" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A129" t="s">
-        <v>327</v>
-      </c>
-      <c r="B129" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="130" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A130" t="s">
-        <v>328</v>
-      </c>
-      <c r="B130" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="131" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A131" s="1" t="s">
-        <v>329</v>
-      </c>
-      <c r="B131" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="132" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A132" s="1" t="s">
-        <v>330</v>
-      </c>
-      <c r="B132" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="133" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A133" s="1" t="s">
-        <v>337</v>
-      </c>
-      <c r="B133" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="134" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A134" s="1" t="s">
-        <v>338</v>
-      </c>
-      <c r="B134" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="135" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A135" s="1" t="s">
-        <v>339</v>
-      </c>
-      <c r="B135" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="136" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A136" t="s">
-        <v>340</v>
-      </c>
-      <c r="B136" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="137" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A137" s="1" t="s">
-        <v>341</v>
-      </c>
-      <c r="B137" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="138" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A138" s="1" t="s">
-        <v>342</v>
-      </c>
-      <c r="B138" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="139" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A139" s="1" t="s">
-        <v>343</v>
-      </c>
-      <c r="B139" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="140" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A140" s="1" t="s">
-        <v>504</v>
-      </c>
-      <c r="B140" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="141" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A141" t="s">
-        <v>505</v>
-      </c>
-      <c r="B141" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="142" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A142" s="1" t="s">
-        <v>506</v>
-      </c>
-      <c r="B142" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="143" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A143" s="1" t="s">
-        <v>507</v>
-      </c>
-      <c r="B143" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="144" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A144" t="s">
-        <v>508</v>
-      </c>
-      <c r="B144" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="145" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A145" s="1" t="s">
-        <v>509</v>
-      </c>
-      <c r="B145" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="146" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A146" s="1" t="s">
-        <v>510</v>
-      </c>
-      <c r="B146" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="147" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A147" s="1" t="s">
-        <v>511</v>
-      </c>
-      <c r="B147" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="148" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A148" t="s">
-        <v>512</v>
-      </c>
-      <c r="B148" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="149" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A149" t="s">
-        <v>513</v>
-      </c>
-      <c r="B149" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="150" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A150" s="1" t="s">
-        <v>514</v>
-      </c>
-      <c r="B150" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="151" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A151" s="1" t="s">
-        <v>515</v>
-      </c>
-      <c r="B151" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="152" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A152" t="s">
-        <v>516</v>
-      </c>
-      <c r="B152" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="153" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A153" s="1" t="s">
-        <v>517</v>
-      </c>
-      <c r="B153" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="154" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A154" s="1" t="s">
-        <v>518</v>
-      </c>
-      <c r="B154" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="155" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A155" s="1" t="s">
-        <v>519</v>
-      </c>
-      <c r="B155" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="156" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A156" s="1" t="s">
-        <v>520</v>
-      </c>
-      <c r="B156" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="157" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A157" s="1" t="s">
-        <v>521</v>
-      </c>
-      <c r="B157" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="158" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="158" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A158" s="1" t="s">
-        <v>522</v>
+        <v>599</v>
       </c>
       <c r="B158" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="159" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A159" s="1" t="s">
-        <v>523</v>
+        <v>7</v>
+      </c>
+      <c r="C158">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="159" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A159" t="s">
+        <v>600</v>
       </c>
       <c r="B159" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="160" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A160" s="1" t="s">
-        <v>524</v>
+        <v>7</v>
+      </c>
+      <c r="C159">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="160" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A160" t="s">
+        <v>601</v>
       </c>
       <c r="B160" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="161" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A161" t="s">
-        <v>525</v>
+        <v>7</v>
+      </c>
+      <c r="C160">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="161" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A161" s="1" t="s">
+        <v>602</v>
       </c>
       <c r="B161" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="162" spans="1:2" x14ac:dyDescent="0.35">
+        <v>7</v>
+      </c>
+      <c r="C161">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="162" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A162" s="1" t="s">
-        <v>526</v>
+        <v>603</v>
       </c>
       <c r="B162" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="163" spans="1:2" x14ac:dyDescent="0.35">
+        <v>7</v>
+      </c>
+      <c r="C162">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="163" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A163" s="1" t="s">
-        <v>527</v>
+        <v>604</v>
       </c>
       <c r="B163" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="164" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A164" s="1" t="s">
-        <v>528</v>
+        <v>7</v>
+      </c>
+      <c r="C163">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="164" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A164" t="s">
+        <v>605</v>
       </c>
       <c r="B164" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="165" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A165" s="1" t="s">
-        <v>529</v>
+        <v>7</v>
+      </c>
+      <c r="C164">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="165" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A165" t="s">
+        <v>606</v>
       </c>
       <c r="B165" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="166" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A166" s="1" t="s">
-        <v>530</v>
-      </c>
-      <c r="B166" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="167" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A167" t="s">
-        <v>581</v>
-      </c>
-      <c r="B167" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="168" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A168" t="s">
-        <v>582</v>
-      </c>
-      <c r="B168" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="169" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A169" t="s">
-        <v>583</v>
-      </c>
-      <c r="B169" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="170" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A170" t="s">
-        <v>584</v>
-      </c>
-      <c r="B170" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="171" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A171" t="s">
-        <v>585</v>
-      </c>
-      <c r="B171" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="172" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A172" s="1" t="s">
-        <v>586</v>
-      </c>
-      <c r="B172" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="173" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A173" s="1" t="s">
-        <v>587</v>
-      </c>
-      <c r="B173" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="174" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A174" t="s">
-        <v>588</v>
-      </c>
-      <c r="B174" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="175" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A175" s="1" t="s">
-        <v>589</v>
-      </c>
-      <c r="B175" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="176" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A176" s="1" t="s">
-        <v>590</v>
-      </c>
-      <c r="B176" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="177" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A177" s="1" t="s">
-        <v>591</v>
-      </c>
-      <c r="B177" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="178" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A178" t="s">
-        <v>592</v>
-      </c>
-      <c r="B178" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="179" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A179" t="s">
-        <v>593</v>
-      </c>
-      <c r="B179" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="180" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A180" t="s">
-        <v>594</v>
-      </c>
-      <c r="B180" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="181" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A181" s="1" t="s">
-        <v>595</v>
-      </c>
-      <c r="B181" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="182" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A182" s="1" t="s">
-        <v>596</v>
-      </c>
-      <c r="B182" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="183" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A183" s="1" t="s">
-        <v>597</v>
-      </c>
-      <c r="B183" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="184" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A184" s="1" t="s">
-        <v>598</v>
-      </c>
-      <c r="B184" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="185" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A185" s="1" t="s">
-        <v>599</v>
-      </c>
-      <c r="B185" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="186" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A186" t="s">
-        <v>600</v>
-      </c>
-      <c r="B186" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="187" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A187" t="s">
-        <v>601</v>
-      </c>
-      <c r="B187" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="188" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A188" s="1" t="s">
-        <v>602</v>
-      </c>
-      <c r="B188" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="189" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A189" s="1" t="s">
-        <v>603</v>
-      </c>
-      <c r="B189" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="190" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A190" s="1" t="s">
-        <v>604</v>
-      </c>
-      <c r="B190" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="191" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A191" t="s">
-        <v>605</v>
-      </c>
-      <c r="B191" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="192" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A192" t="s">
-        <v>606</v>
-      </c>
-      <c r="B192" t="s">
-        <v>7</v>
-      </c>
+      <c r="C165">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="171" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A171" s="1"/>
+    </row>
+    <row r="172" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A172" s="1"/>
+    </row>
+    <row r="173" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A173" s="1"/>
+    </row>
+    <row r="174" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A174" s="1"/>
+    </row>
+    <row r="176" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A176" s="1"/>
+    </row>
+    <row r="177" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A177" s="1"/>
+    </row>
+    <row r="178" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A178" s="1"/>
+    </row>
+    <row r="179" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A179" s="1"/>
+    </row>
+    <row r="180" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A180" s="1"/>
+    </row>
+    <row r="181" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A181" s="1"/>
+    </row>
+    <row r="183" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A183" s="1"/>
+    </row>
+    <row r="184" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A184" s="1"/>
+    </row>
+    <row r="185" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A185" s="1"/>
+    </row>
+    <row r="186" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A186" s="1"/>
+    </row>
+    <row r="188" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A188" s="1"/>
+    </row>
+    <row r="189" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A189" s="1"/>
+    </row>
+    <row r="191" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A191" s="1"/>
+    </row>
+    <row r="192" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A192" s="1"/>
     </row>
     <row r="193" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A193" s="1"/>
@@ -10470,6 +10809,9 @@
     <row r="196" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A196" s="1"/>
     </row>
+    <row r="197" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A197" s="1"/>
+    </row>
     <row r="198" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A198" s="1"/>
     </row>
@@ -10488,18 +10830,18 @@
     <row r="203" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A203" s="1"/>
     </row>
+    <row r="204" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A204" s="1"/>
+    </row>
     <row r="205" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A205" s="1"/>
     </row>
-    <row r="206" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A206" s="1"/>
-    </row>
-    <row r="207" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A207" s="1"/>
-    </row>
     <row r="208" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A208" s="1"/>
     </row>
+    <row r="209" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A209" s="1"/>
+    </row>
     <row r="210" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A210" s="1"/>
     </row>
@@ -10524,18 +10866,12 @@
     <row r="218" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A218" s="1"/>
     </row>
-    <row r="219" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A219" s="1"/>
-    </row>
     <row r="220" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A220" s="1"/>
     </row>
     <row r="221" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A221" s="1"/>
     </row>
-    <row r="222" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A222" s="1"/>
-    </row>
     <row r="223" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A223" s="1"/>
     </row>
@@ -10560,8 +10896,8 @@
     <row r="232" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A232" s="1"/>
     </row>
-    <row r="233" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A233" s="1"/>
+    <row r="234" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A234" s="1"/>
     </row>
     <row r="235" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A235" s="1"/>
@@ -10581,12 +10917,18 @@
     <row r="240" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A240" s="1"/>
     </row>
+    <row r="241" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A241" s="1"/>
+    </row>
     <row r="242" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A242" s="1"/>
     </row>
     <row r="243" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A243" s="1"/>
     </row>
+    <row r="244" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A244" s="1"/>
+    </row>
     <row r="245" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A245" s="1"/>
     </row>
@@ -10602,17 +10944,17 @@
     <row r="249" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A249" s="1"/>
     </row>
-    <row r="252" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A252" s="1"/>
-    </row>
-    <row r="253" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A253" s="1"/>
+    <row r="250" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A250" s="1"/>
+    </row>
+    <row r="251" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A251" s="1"/>
     </row>
     <row r="254" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A254" s="1"/>
     </row>
-    <row r="256" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A256" s="1"/>
+    <row r="255" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A255" s="1"/>
     </row>
     <row r="257" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A257" s="1"/>
@@ -10638,95 +10980,86 @@
     <row r="264" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A264" s="1"/>
     </row>
-    <row r="265" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A265" s="1"/>
-    </row>
-    <row r="266" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A266" s="1"/>
-    </row>
-    <row r="267" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A267" s="1"/>
-    </row>
     <row r="268" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A268" s="1"/>
     </row>
     <row r="269" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A269" s="1"/>
     </row>
-    <row r="270" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A270" s="1"/>
-    </row>
-    <row r="271" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A271" s="1"/>
-    </row>
-    <row r="272" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A272" s="1"/>
-    </row>
-    <row r="273" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A273" s="1"/>
-    </row>
-    <row r="276" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A276" s="1"/>
-    </row>
-    <row r="277" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A277" s="1"/>
-    </row>
-    <row r="279" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A279" s="1"/>
-    </row>
-    <row r="280" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A280" s="1"/>
-    </row>
-    <row r="281" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A281" s="1"/>
-    </row>
-    <row r="282" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A282" s="1"/>
-    </row>
-    <row r="283" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A283" s="1"/>
-    </row>
-    <row r="284" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A284" s="1"/>
-    </row>
-    <row r="285" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A285" s="1"/>
-    </row>
-    <row r="286" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A286" s="1"/>
-    </row>
-    <row r="290" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A290" s="1"/>
-    </row>
-    <row r="291" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A291" s="1"/>
-    </row>
-    <row r="296" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A296" s="1"/>
+    <row r="274" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A274" s="1"/>
+    </row>
+    <row r="275" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A275" s="1"/>
+    </row>
+    <row r="294" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A294" s="1"/>
+    </row>
+    <row r="295" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A295" s="1"/>
     </row>
     <row r="297" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A297" s="1"/>
     </row>
+    <row r="298" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A298" s="1"/>
+    </row>
+    <row r="299" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A299" s="1"/>
+    </row>
+    <row r="300" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A300" s="1"/>
+    </row>
+    <row r="301" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A301" s="1"/>
+    </row>
+    <row r="304" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A304" s="1"/>
+    </row>
+    <row r="305" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A305" s="1"/>
+    </row>
+    <row r="307" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A307" s="1"/>
+    </row>
+    <row r="308" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A308" s="1"/>
+    </row>
+    <row r="310" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A310" s="1"/>
+    </row>
+    <row r="311" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A311" s="1"/>
+    </row>
+    <row r="312" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A312" s="1"/>
+    </row>
+    <row r="313" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A313" s="1"/>
+    </row>
+    <row r="315" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A315" s="1"/>
+    </row>
     <row r="316" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A316" s="1"/>
     </row>
-    <row r="317" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A317" s="1"/>
+    <row r="318" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A318" s="1"/>
     </row>
     <row r="319" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A319" s="1"/>
     </row>
-    <row r="320" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A320" s="1"/>
-    </row>
     <row r="321" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A321" s="1"/>
     </row>
     <row r="322" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A322" s="1"/>
     </row>
-    <row r="323" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A323" s="1"/>
+    <row r="324" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A324" s="1"/>
+    </row>
+    <row r="325" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A325" s="1"/>
     </row>
     <row r="326" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A326" s="1"/>
@@ -10734,30 +11067,15 @@
     <row r="327" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A327" s="1"/>
     </row>
+    <row r="328" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A328" s="1"/>
+    </row>
     <row r="329" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A329" s="1"/>
     </row>
     <row r="330" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A330" s="1"/>
     </row>
-    <row r="332" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A332" s="1"/>
-    </row>
-    <row r="333" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A333" s="1"/>
-    </row>
-    <row r="334" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A334" s="1"/>
-    </row>
-    <row r="335" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A335" s="1"/>
-    </row>
-    <row r="337" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A337" s="1"/>
-    </row>
-    <row r="338" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A338" s="1"/>
-    </row>
     <row r="340" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A340" s="1"/>
     </row>
@@ -10770,47 +11088,32 @@
     <row r="344" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A344" s="1"/>
     </row>
+    <row r="345" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A345" s="1"/>
+    </row>
     <row r="346" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A346" s="1"/>
     </row>
     <row r="347" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A347" s="1"/>
     </row>
-    <row r="348" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A348" s="1"/>
-    </row>
-    <row r="349" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A349" s="1"/>
-    </row>
-    <row r="350" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A350" s="1"/>
-    </row>
     <row r="351" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A351" s="1"/>
     </row>
     <row r="352" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A352" s="1"/>
     </row>
-    <row r="362" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A362" s="1"/>
-    </row>
-    <row r="363" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A363" s="1"/>
-    </row>
-    <row r="365" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A365" s="1"/>
-    </row>
-    <row r="366" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A366" s="1"/>
-    </row>
-    <row r="367" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A367" s="1"/>
-    </row>
-    <row r="368" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A368" s="1"/>
-    </row>
-    <row r="369" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A369" s="1"/>
+    <row r="353" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A353" s="1"/>
+    </row>
+    <row r="356" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A356" s="1"/>
+    </row>
+    <row r="357" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A357" s="1"/>
+    </row>
+    <row r="372" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A372" s="1"/>
     </row>
     <row r="373" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A373" s="1"/>
@@ -10818,29 +11121,53 @@
     <row r="374" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A374" s="1"/>
     </row>
-    <row r="375" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A375" s="1"/>
-    </row>
-    <row r="378" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A378" s="1"/>
+    <row r="376" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A376" s="1"/>
+    </row>
+    <row r="377" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A377" s="1"/>
     </row>
     <row r="379" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A379" s="1"/>
     </row>
-    <row r="394" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A394" s="1"/>
-    </row>
-    <row r="395" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A395" s="1"/>
+    <row r="380" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A380" s="1"/>
+    </row>
+    <row r="381" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A381" s="1"/>
+    </row>
+    <row r="384" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A384" s="1"/>
+    </row>
+    <row r="385" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A385" s="1"/>
+    </row>
+    <row r="386" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A386" s="1"/>
+    </row>
+    <row r="388" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A388" s="1"/>
+    </row>
+    <row r="389" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A389" s="1"/>
+    </row>
+    <row r="391" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A391" s="1"/>
+    </row>
+    <row r="392" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A392" s="1"/>
+    </row>
+    <row r="393" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A393" s="1"/>
     </row>
     <row r="396" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A396" s="1"/>
     </row>
-    <row r="398" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A398" s="1"/>
-    </row>
-    <row r="399" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A399" s="1"/>
+    <row r="397" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A397" s="1"/>
+    </row>
+    <row r="400" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A400" s="1"/>
     </row>
     <row r="401" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A401" s="1"/>
@@ -10851,30 +11178,30 @@
     <row r="403" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A403" s="1"/>
     </row>
+    <row r="405" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A405" s="1"/>
+    </row>
     <row r="406" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A406" s="1"/>
     </row>
-    <row r="407" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A407" s="1"/>
-    </row>
     <row r="408" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A408" s="1"/>
     </row>
-    <row r="410" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A410" s="1"/>
+    <row r="409" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A409" s="1"/>
     </row>
     <row r="411" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A411" s="1"/>
     </row>
-    <row r="413" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A413" s="1"/>
-    </row>
-    <row r="414" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A414" s="1"/>
+    <row r="412" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A412" s="1"/>
     </row>
     <row r="415" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A415" s="1"/>
     </row>
+    <row r="416" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A416" s="1"/>
+    </row>
     <row r="418" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A418" s="1"/>
     </row>
@@ -10887,47 +11214,44 @@
     <row r="423" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A423" s="1"/>
     </row>
-    <row r="424" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A424" s="1"/>
-    </row>
-    <row r="425" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A425" s="1"/>
+    <row r="426" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A426" s="1"/>
     </row>
     <row r="427" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A427" s="1"/>
     </row>
-    <row r="428" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A428" s="1"/>
-    </row>
-    <row r="430" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A430" s="1"/>
-    </row>
     <row r="431" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A431" s="1"/>
     </row>
-    <row r="433" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A433" s="1"/>
-    </row>
-    <row r="434" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A434" s="1"/>
-    </row>
-    <row r="437" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A437" s="1"/>
+    <row r="432" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A432" s="1"/>
+    </row>
+    <row r="435" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A435" s="1"/>
+    </row>
+    <row r="436" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A436" s="1"/>
     </row>
     <row r="438" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A438" s="1"/>
     </row>
+    <row r="439" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A439" s="1"/>
+    </row>
     <row r="440" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A440" s="1"/>
     </row>
-    <row r="441" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A441" s="1"/>
+    <row r="443" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A443" s="1"/>
     </row>
     <row r="444" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A444" s="1"/>
     </row>
-    <row r="445" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A445" s="1"/>
+    <row r="446" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A446" s="1"/>
+    </row>
+    <row r="447" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A447" s="1"/>
     </row>
     <row r="448" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A448" s="1"/>
@@ -10935,20 +11259,23 @@
     <row r="449" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A449" s="1"/>
     </row>
-    <row r="453" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A453" s="1"/>
-    </row>
-    <row r="454" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A454" s="1"/>
-    </row>
-    <row r="457" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A457" s="1"/>
+    <row r="451" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A451" s="1"/>
+    </row>
+    <row r="452" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A452" s="1"/>
+    </row>
+    <row r="455" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A455" s="1"/>
+    </row>
+    <row r="456" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A456" s="1"/>
     </row>
     <row r="458" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A458" s="1"/>
     </row>
-    <row r="460" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A460" s="1"/>
+    <row r="459" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A459" s="1"/>
     </row>
     <row r="461" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A461" s="1"/>
@@ -10956,15 +11283,12 @@
     <row r="462" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A462" s="1"/>
     </row>
+    <row r="464" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A464" s="1"/>
+    </row>
     <row r="465" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A465" s="1"/>
     </row>
-    <row r="466" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A466" s="1"/>
-    </row>
-    <row r="468" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A468" s="1"/>
-    </row>
     <row r="469" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A469" s="1"/>
     </row>
@@ -10974,47 +11298,41 @@
     <row r="471" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A471" s="1"/>
     </row>
+    <row r="472" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A472" s="1"/>
+    </row>
     <row r="473" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A473" s="1"/>
     </row>
     <row r="474" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A474" s="1"/>
     </row>
-    <row r="477" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A477" s="1"/>
-    </row>
     <row r="478" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A478" s="1"/>
     </row>
+    <row r="479" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A479" s="1"/>
+    </row>
     <row r="480" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A480" s="1"/>
     </row>
-    <row r="481" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A481" s="1"/>
+    <row r="482" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A482" s="1"/>
     </row>
     <row r="483" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A483" s="1"/>
     </row>
-    <row r="484" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A484" s="1"/>
+    <row r="485" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A485" s="1"/>
     </row>
     <row r="486" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A486" s="1"/>
     </row>
-    <row r="487" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A487" s="1"/>
-    </row>
-    <row r="491" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A491" s="1"/>
-    </row>
-    <row r="492" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A492" s="1"/>
-    </row>
-    <row r="493" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A493" s="1"/>
-    </row>
-    <row r="494" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A494" s="1"/>
+    <row r="489" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A489" s="1"/>
+    </row>
+    <row r="490" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A490" s="1"/>
     </row>
     <row r="495" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A495" s="1"/>
@@ -11022,15 +11340,18 @@
     <row r="496" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A496" s="1"/>
     </row>
-    <row r="500" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A500" s="1"/>
-    </row>
-    <row r="501" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A501" s="1"/>
+    <row r="497" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A497" s="1"/>
+    </row>
+    <row r="498" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A498" s="1"/>
     </row>
     <row r="502" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A502" s="1"/>
     </row>
+    <row r="503" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A503" s="1"/>
+    </row>
     <row r="504" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A504" s="1"/>
     </row>
@@ -11043,12 +11364,24 @@
     <row r="508" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A508" s="1"/>
     </row>
+    <row r="509" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A509" s="1"/>
+    </row>
     <row r="511" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A511" s="1"/>
     </row>
     <row r="512" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A512" s="1"/>
     </row>
+    <row r="514" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A514" s="1"/>
+    </row>
+    <row r="515" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A515" s="1"/>
+    </row>
+    <row r="516" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A516" s="1"/>
+    </row>
     <row r="517" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A517" s="1"/>
     </row>
@@ -11061,6 +11394,12 @@
     <row r="520" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A520" s="1"/>
     </row>
+    <row r="522" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A522" s="1"/>
+    </row>
+    <row r="523" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A523" s="1"/>
+    </row>
     <row r="524" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A524" s="1"/>
     </row>
@@ -11073,21 +11412,27 @@
     <row r="527" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A527" s="1"/>
     </row>
+    <row r="528" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A528" s="1"/>
+    </row>
     <row r="529" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A529" s="1"/>
     </row>
-    <row r="530" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A530" s="1"/>
-    </row>
     <row r="531" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A531" s="1"/>
     </row>
+    <row r="532" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A532" s="1"/>
+    </row>
     <row r="533" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A533" s="1"/>
     </row>
     <row r="534" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A534" s="1"/>
     </row>
+    <row r="535" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A535" s="1"/>
+    </row>
     <row r="536" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A536" s="1"/>
     </row>
@@ -11097,30 +11442,6 @@
     <row r="538" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A538" s="1"/>
     </row>
-    <row r="539" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A539" s="1"/>
-    </row>
-    <row r="540" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A540" s="1"/>
-    </row>
-    <row r="541" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A541" s="1"/>
-    </row>
-    <row r="542" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A542" s="1"/>
-    </row>
-    <row r="544" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A544" s="1"/>
-    </row>
-    <row r="545" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A545" s="1"/>
-    </row>
-    <row r="546" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A546" s="1"/>
-    </row>
-    <row r="547" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A547" s="1"/>
-    </row>
     <row r="548" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A548" s="1"/>
     </row>
@@ -11139,54 +11460,14 @@
     <row r="554" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A554" s="1"/>
     </row>
-    <row r="555" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A555" s="1"/>
-    </row>
-    <row r="556" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A556" s="1"/>
-    </row>
-    <row r="557" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A557" s="1"/>
-    </row>
-    <row r="558" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A558" s="1"/>
-    </row>
-    <row r="559" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A559" s="1"/>
-    </row>
-    <row r="560" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A560" s="1"/>
-    </row>
-    <row r="570" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A570" s="1"/>
-    </row>
-    <row r="571" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A571" s="1"/>
-    </row>
-    <row r="572" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A572" s="1"/>
-    </row>
-    <row r="573" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A573" s="1"/>
-    </row>
-    <row r="575" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A575" s="1"/>
-    </row>
-    <row r="576" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A576" s="1"/>
-    </row>
-    <row r="587" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A587" s="1"/>
-    </row>
-    <row r="588" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A588" s="1"/>
+    <row r="565" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A565" s="1"/>
+    </row>
+    <row r="566" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A566" s="1"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:B588" xr:uid="{027D69F3-84A9-42C0-BBC6-9B3F4DA908D0}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B588">
-      <sortCondition ref="B1:B588"/>
-    </sortState>
-  </autoFilter>
+  <autoFilter ref="A1:C165" xr:uid="{E249DB83-0A84-4589-AA81-D14C1D72E018}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>